<commit_message>
added health facility to user model
</commit_message>
<xml_diff>
--- a/GetInBundibugyoUsers.xlsx
+++ b/GetInBundibugyoUsers.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="122">
   <si>
     <t xml:space="preserve">Observations</t>
   </si>
@@ -115,30 +115,45 @@
     <t xml:space="preserve">male</t>
   </si>
   <si>
+    <t xml:space="preserve">Kisubba HC III</t>
+  </si>
+  <si>
     <t xml:space="preserve">Happy Ham</t>
   </si>
   <si>
     <t xml:space="preserve">Salongo</t>
   </si>
   <si>
+    <t xml:space="preserve">KIsubba HC III</t>
+  </si>
+  <si>
     <t xml:space="preserve">Monday</t>
   </si>
   <si>
     <t xml:space="preserve">Robert</t>
   </si>
   <si>
+    <t xml:space="preserve">Gadaffi HC II</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ajuna</t>
   </si>
   <si>
     <t xml:space="preserve">Clernsow</t>
   </si>
   <si>
+    <t xml:space="preserve">Bubukwanga HC III</t>
+  </si>
+  <si>
     <t xml:space="preserve">Byamaka</t>
   </si>
   <si>
     <t xml:space="preserve">Doe</t>
   </si>
   <si>
+    <t xml:space="preserve">Bundibugyo Hospital</t>
+  </si>
+  <si>
     <t xml:space="preserve">Edson</t>
   </si>
   <si>
@@ -160,12 +175,18 @@
     <t xml:space="preserve">Manda</t>
   </si>
   <si>
+    <t xml:space="preserve">Ebenezer HC III</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bahumawe</t>
   </si>
   <si>
     <t xml:space="preserve">James</t>
   </si>
   <si>
+    <t xml:space="preserve">Bukangama HC III</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nyambusa</t>
   </si>
   <si>
@@ -193,18 +214,27 @@
     <t xml:space="preserve">Florence</t>
   </si>
   <si>
+    <t xml:space="preserve">Kikyo IV</t>
+  </si>
+  <si>
     <t xml:space="preserve">Katusabe Nsunga</t>
   </si>
   <si>
     <t xml:space="preserve">Dolice</t>
   </si>
   <si>
+    <t xml:space="preserve">Kakuka HC III</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rosemary</t>
   </si>
   <si>
     <t xml:space="preserve">Katusabe</t>
   </si>
   <si>
+    <t xml:space="preserve">Nyahuka HC IV</t>
+  </si>
+  <si>
     <t xml:space="preserve">Baguma</t>
   </si>
   <si>
@@ -214,6 +244,9 @@
     <t xml:space="preserve">Kansiime</t>
   </si>
   <si>
+    <t xml:space="preserve">Kima HC III</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kabugho</t>
   </si>
   <si>
@@ -238,12 +271,18 @@
     <t xml:space="preserve">Steven</t>
   </si>
   <si>
+    <t xml:space="preserve">Butama HC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Friday </t>
   </si>
   <si>
     <t xml:space="preserve">Peter</t>
   </si>
   <si>
+    <t xml:space="preserve">Busunga HC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Byahuriuenda</t>
   </si>
   <si>
@@ -268,6 +307,9 @@
     <t xml:space="preserve">Fred</t>
   </si>
   <si>
+    <t xml:space="preserve">Burondo HC III</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bataga</t>
   </si>
   <si>
@@ -295,6 +337,9 @@
     <t xml:space="preserve">Ndyanabo</t>
   </si>
   <si>
+    <t xml:space="preserve">Busaru HC IV</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kyaligonza</t>
   </si>
   <si>
@@ -313,6 +358,9 @@
     <t xml:space="preserve">Getrude</t>
   </si>
   <si>
+    <t xml:space="preserve">Ngamba HC II</t>
+  </si>
+  <si>
     <t xml:space="preserve">Baluku</t>
   </si>
   <si>
@@ -335,6 +383,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ngume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ntandi HC III</t>
   </si>
   <si>
     <t xml:space="preserve">Kabukalhese</t>
@@ -371,7 +422,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -413,12 +464,6 @@
       <name val="Gill Sans"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -491,11 +536,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -776,10 +821,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -811,13 +856,16 @@
       <c r="F1" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>779779508</v>
@@ -831,13 +879,16 @@
       <c r="F2" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G2" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>786429831</v>
@@ -851,13 +902,16 @@
       <c r="F3" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>775100813</v>
@@ -871,13 +925,16 @@
       <c r="F4" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>785103594</v>
@@ -891,13 +948,16 @@
       <c r="F5" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>779368391</v>
@@ -911,13 +971,16 @@
       <c r="F6" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>774783370</v>
@@ -931,13 +994,16 @@
       <c r="F7" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>777121818</v>
@@ -951,13 +1017,16 @@
       <c r="F8" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G8" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>786282955</v>
@@ -971,13 +1040,16 @@
       <c r="F9" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>774306089</v>
@@ -991,13 +1063,16 @@
       <c r="F10" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G10" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>771629813</v>
@@ -1006,18 +1081,21 @@
         <v>785749813</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>773787281</v>
@@ -1031,13 +1109,16 @@
       <c r="F12" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G12" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>789222153</v>
@@ -1046,18 +1127,21 @@
         <v>785734687</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>787560024</v>
@@ -1066,18 +1150,21 @@
         <v>785738759</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>782580805</v>
@@ -1086,18 +1173,21 @@
         <v>785731965</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>781030201</v>
@@ -1106,18 +1196,21 @@
         <v>785743265</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C17" s="4" t="n">
         <v>773565997</v>
@@ -1131,13 +1224,16 @@
       <c r="F17" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G17" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>774071441</v>
@@ -1151,13 +1247,16 @@
       <c r="F18" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G18" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>786617214</v>
@@ -1171,13 +1270,16 @@
       <c r="F19" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G19" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>775287097</v>
@@ -1191,13 +1293,16 @@
       <c r="F20" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G20" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C21" s="4" t="n">
         <v>788435493</v>
@@ -1211,13 +1316,16 @@
       <c r="F21" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G21" s="4" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C22" s="4" t="n">
         <v>779779512</v>
@@ -1231,13 +1339,16 @@
       <c r="F22" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G22" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C23" s="4" t="n">
         <v>772268781</v>
@@ -1251,13 +1362,16 @@
       <c r="F23" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G23" s="4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C24" s="4" t="n">
         <v>789123881</v>
@@ -1271,13 +1385,16 @@
       <c r="F24" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C25" s="4" t="n">
         <v>774950906</v>
@@ -1291,13 +1408,16 @@
       <c r="F25" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G25" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C26" s="4" t="n">
         <v>774797842</v>
@@ -1306,18 +1426,21 @@
         <v>785746925</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>21</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="C27" s="4" t="n">
         <v>778791719</v>
@@ -1331,13 +1454,16 @@
       <c r="F27" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G27" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C28" s="4" t="n">
         <v>781983529</v>
@@ -1351,13 +1477,16 @@
       <c r="F28" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G28" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C29" s="4" t="n">
         <v>788714945</v>
@@ -1371,13 +1500,16 @@
       <c r="F29" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G29" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="C30" s="4" t="n">
         <v>779553931</v>
@@ -1386,18 +1518,21 @@
         <v>783567349</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C31" s="4" t="n">
         <v>782417325</v>
@@ -1406,18 +1541,21 @@
         <v>785731402</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>21</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C32" s="4" t="n">
         <v>788445583</v>
@@ -1431,13 +1569,16 @@
       <c r="F32" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G32" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="C33" s="4" t="n">
         <v>785493932</v>
@@ -1451,13 +1592,16 @@
       <c r="F33" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G33" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="C34" s="4" t="n">
         <v>784067144</v>
@@ -1471,13 +1615,16 @@
       <c r="F34" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G34" s="4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="C35" s="4" t="n">
         <v>786133034</v>
@@ -1491,13 +1638,16 @@
       <c r="F35" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G35" s="4" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="C36" s="4" t="n">
         <v>771830353</v>
@@ -1511,13 +1661,16 @@
       <c r="F36" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G36" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="C37" s="4" t="n">
         <v>782842685</v>
@@ -1526,18 +1679,21 @@
         <v>785675185</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C38" s="4" t="n">
         <v>789611486</v>
@@ -1546,18 +1702,21 @@
         <v>785736254</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C39" s="4" t="n">
         <v>783853862</v>
@@ -1566,18 +1725,21 @@
         <v>783484105</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="C40" s="4" t="n">
         <v>779779435</v>
@@ -1591,13 +1753,16 @@
       <c r="F40" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G40" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="C41" s="4" t="n">
         <v>779779399</v>
@@ -1611,13 +1776,16 @@
       <c r="F41" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G41" s="4" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="C42" s="4" t="n">
         <v>786422111</v>
@@ -1626,18 +1794,21 @@
         <v>785745918</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>21</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C43" s="4" t="n">
         <v>783587006</v>
@@ -1649,15 +1820,18 @@
         <v>20</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="C44" s="4" t="n">
         <v>774728733</v>
@@ -1666,7 +1840,7 @@
         <v>785762185</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>21</v>
@@ -1674,10 +1848,10 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C45" s="6" t="n">
         <v>783587006</v>
@@ -1689,7 +1863,7 @@
         <v>20</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>